<commit_message>
Chnaged the file location paths
</commit_message>
<xml_diff>
--- a/UserProfile/excel/omkar.xlsx
+++ b/UserProfile/excel/omkar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/traderscafe/Documents/TradeMan/Utils/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/traderscafe/Desktop/Main/TradeMan/UserProfile/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B09A864-AE11-9648-A058-BC3A0D9C6D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9930D9DE-32EC-C246-8F9C-087BD125DC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="26600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="118">
   <si>
     <t>Tr.No</t>
   </si>
@@ -303,10 +303,19 @@
     <t>14:20</t>
   </si>
   <si>
-    <t>44100</t>
-  </si>
-  <si>
-    <t>19600</t>
+    <t>45500</t>
+  </si>
+  <si>
+    <t>11:02</t>
+  </si>
+  <si>
+    <t>20300</t>
+  </si>
+  <si>
+    <t>11:04</t>
+  </si>
+  <si>
+    <t>12:39</t>
   </si>
   <si>
     <t>Trade Type</t>
@@ -346,6 +355,9 @@
   </si>
   <si>
     <t>11:36</t>
+  </si>
+  <si>
+    <t>10:06</t>
   </si>
   <si>
     <t>Trade_Type</t>
@@ -1103,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1633,11 +1645,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2545,10 +2555,10 @@
       <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="C25">
+        <v>44100</v>
+      </c>
+      <c r="D25" s="2">
         <v>45161</v>
       </c>
       <c r="E25" t="s">
@@ -2583,10 +2593,10 @@
       <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26">
+        <v>19600</v>
+      </c>
+      <c r="D26" s="2">
         <v>45161</v>
       </c>
       <c r="E26" t="s">
@@ -2612,6 +2622,82 @@
       </c>
       <c r="L26">
         <v>331.02826240000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45182</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27">
+        <v>117.91578947000001</v>
+      </c>
+      <c r="H27">
+        <v>397.32</v>
+      </c>
+      <c r="I27">
+        <v>279.40421053</v>
+      </c>
+      <c r="J27">
+        <v>285</v>
+      </c>
+      <c r="K27">
+        <v>79630.200001050005</v>
+      </c>
+      <c r="L27">
+        <v>285.46153171728088</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45182</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28">
+        <v>111.99</v>
+      </c>
+      <c r="H28">
+        <v>150</v>
+      </c>
+      <c r="I28">
+        <v>38.010000000000012</v>
+      </c>
+      <c r="J28">
+        <v>960</v>
+      </c>
+      <c r="K28">
+        <v>36489.600000000013</v>
+      </c>
+      <c r="L28">
+        <v>271.16723200000001</v>
       </c>
     </row>
   </sheetData>
@@ -2621,13 +2707,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2637,7 +2724,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>40</v>
@@ -2658,10 +2745,10 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>44</v>
@@ -2678,13 +2765,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D2">
         <v>19500</v>
@@ -2693,10 +2780,10 @@
         <v>45142</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H2">
         <v>205.95</v>
@@ -2716,13 +2803,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D3">
         <v>19600</v>
@@ -2731,10 +2818,10 @@
         <v>45145</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H3">
         <v>170.61</v>
@@ -2754,13 +2841,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D4">
         <v>19600</v>
@@ -2769,10 +2856,10 @@
         <v>45146</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H4">
         <v>154.31</v>
@@ -2801,13 +2888,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D5">
         <v>19500</v>
@@ -2816,10 +2903,10 @@
         <v>45147</v>
       </c>
       <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
         <v>103</v>
-      </c>
-      <c r="G5" t="s">
-        <v>100</v>
       </c>
       <c r="H5">
         <v>125.68</v>
@@ -2848,13 +2935,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D6">
         <v>19600</v>
@@ -2863,10 +2950,10 @@
         <v>45148</v>
       </c>
       <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
         <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>100</v>
       </c>
       <c r="H6">
         <v>105.4875</v>
@@ -2895,13 +2982,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D7">
         <v>19500</v>
@@ -2910,10 +2997,10 @@
         <v>45149</v>
       </c>
       <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" t="s">
         <v>103</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
       </c>
       <c r="H7">
         <v>191.61</v>
@@ -2942,13 +3029,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D8">
         <v>19300</v>
@@ -2957,10 +3044,10 @@
         <v>45152</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H8">
         <v>169.99</v>
@@ -2989,13 +3076,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>19300</v>
@@ -3004,10 +3091,10 @@
         <v>45154</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H9">
         <v>121.46250000000001</v>
@@ -3036,13 +3123,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>19300</v>
@@ -3051,10 +3138,10 @@
         <v>45154</v>
       </c>
       <c r="F10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H10">
         <v>121.46250000000001</v>
@@ -3083,13 +3170,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D11">
         <v>19400</v>
@@ -3098,10 +3185,10 @@
         <v>45155</v>
       </c>
       <c r="F11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
         <v>103</v>
-      </c>
-      <c r="G11" t="s">
-        <v>100</v>
       </c>
       <c r="H11">
         <v>91.199999999999989</v>
@@ -3130,13 +3217,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D12">
         <v>19300</v>
@@ -3145,10 +3232,10 @@
         <v>45156</v>
       </c>
       <c r="F12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" t="s">
         <v>103</v>
-      </c>
-      <c r="G12" t="s">
-        <v>100</v>
       </c>
       <c r="H12">
         <v>189.6</v>
@@ -3177,13 +3264,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
         <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D13">
         <v>19300</v>
@@ -3192,10 +3279,10 @@
         <v>45159</v>
       </c>
       <c r="F13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" t="s">
         <v>103</v>
-      </c>
-      <c r="G13" t="s">
-        <v>100</v>
       </c>
       <c r="H13">
         <v>165.00714285999999</v>
@@ -3224,13 +3311,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D14">
         <v>19400</v>
@@ -3239,10 +3326,10 @@
         <v>45160</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H14">
         <v>130.65</v>
@@ -3271,25 +3358,25 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
         <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15">
         <v>19400</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>45161</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H15">
         <v>95.35</v>
@@ -3314,6 +3401,53 @@
       </c>
       <c r="O15">
         <v>244.76290441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16">
+        <v>20000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45182</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16">
+        <v>125.22</v>
+      </c>
+      <c r="I16">
+        <v>135.99</v>
+      </c>
+      <c r="J16">
+        <v>5.05</v>
+      </c>
+      <c r="K16">
+        <v>3.75</v>
+      </c>
+      <c r="L16">
+        <v>-12.070000000000009</v>
+      </c>
+      <c r="M16">
+        <v>450</v>
+      </c>
+      <c r="N16">
+        <v>-5431.5000000000045</v>
+      </c>
+      <c r="O16">
+        <v>273.09381694000001</v>
       </c>
     </row>
   </sheetData>
@@ -3323,35 +3457,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -3362,7 +3494,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -3391,7 +3523,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B3">
         <v>450</v>
@@ -3416,6 +3548,35 @@
       </c>
       <c r="I3">
         <v>1588.7136820550741</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+      <c r="C4">
+        <v>20039.95</v>
+      </c>
+      <c r="D4">
+        <v>20023.91</v>
+      </c>
+      <c r="E4">
+        <v>23.61</v>
+      </c>
+      <c r="F4">
+        <v>26.38</v>
+      </c>
+      <c r="G4">
+        <v>-13.27000000000087</v>
+      </c>
+      <c r="H4">
+        <v>-7962.0000000005239</v>
+      </c>
+      <c r="I4">
+        <v>2129.204157188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>